<commit_message>
figures to illustrate interpolation and D
</commit_message>
<xml_diff>
--- a/bud-leaf-stats_V4.xlsx
+++ b/bud-leaf-stats_V4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="102">
   <si>
     <t>bud</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>sample05 image stack directory does not exist.</t>
-  </si>
-  <si>
-    <t>Voxel size is missing (once the voxel size is added here, the leaf and bud volumes will be correctly displayed.)</t>
   </si>
 </sst>
 </file>
@@ -806,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2765,15 +2762,15 @@
       </c>
       <c r="H46">
         <f>105858*R46^3*(S46*2)^3*0.000000000001</f>
-        <v>0</v>
+        <v>1.4010689454493788E-4</v>
       </c>
       <c r="I46">
         <f>7999942*R46^3*(S46*2)^3*0.000000000001</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1.0588212796006153E-2</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3232345934508026E-2</v>
       </c>
       <c r="K46">
         <v>0.68600000000000005</v>
@@ -2793,11 +2790,11 @@
       <c r="P46">
         <v>0.85099999999999998</v>
       </c>
+      <c r="R46" s="10">
+        <v>5.4897</v>
+      </c>
       <c r="S46">
         <v>1</v>
-      </c>
-      <c r="T46" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:20">

</xml_diff>